<commit_message>
Atualiza Divisão de Atividades
Atualiza Divisão de Atividades
</commit_message>
<xml_diff>
--- a/Documentação/Lista de Atividades e Divisão de Tarefas.xlsx
+++ b/Documentação/Lista de Atividades e Divisão de Tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\avaliacaoprofessoresUFG-master\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\GitHub\avaliacaoprofessoresUFG\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>Atividade</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>Bruno Rodrigues/Ítalo Miranda</t>
+  </si>
+  <si>
+    <t>Cadastro de Docente</t>
+  </si>
+  <si>
+    <t>Ademar Júnior/Jean Lucas/Fernando Gonzaga</t>
+  </si>
+  <si>
+    <t>Cadastro de Atividades</t>
+  </si>
+  <si>
+    <t>Mário Hayasaki/Guilherme Moreno</t>
   </si>
 </sst>
 </file>
@@ -227,10 +239,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,11 +524,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -773,6 +784,28 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>